<commit_message>
Fixed cruise power calculation for mission 2. Removed redundant batteries from database. Changed the order at which calc_cruise calls stuff so that poweratcruise doesnt have to recalculate things. Made new aerofoils from javafoilData actually be used in the master code.
</commit_message>
<xml_diff>
--- a/data/BatterySpecs.xlsx
+++ b/data/BatterySpecs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debna_3tbjgpv\Documents\Design_Build\ADOT2023-main\ADOT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denis\Downloads\ADOT_OO_14_12_2023_1.15_PM\ADOT 2023\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE92B86-E95F-4D91-9E66-557567400327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F812AA-6BA2-4482-9EE3-453DBB20D92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8EC4D84A-1F87-4710-9341-B399FCA76A9C}"/>
+    <workbookView xWindow="16935" yWindow="4260" windowWidth="19680" windowHeight="16395" xr2:uid="{8EC4D84A-1F87-4710-9341-B399FCA76A9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Bh</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Spektrum</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/spektrum-smart-1800mah-22-2v-6s-50c-lipo-battery-ic3.html</t>
-  </si>
-  <si>
     <t>Dualsky</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/dualsky-1800mah-6s-hed-lipo-battery-50c.html</t>
-  </si>
-  <si>
     <t>https://www.modelflight.com.au/dualsky-1250mah-6s-hed-lipo-battery-50c.html</t>
   </si>
   <si>
@@ -74,48 +68,21 @@
     <t>https://www.modelflight.com.au/prime-rc-1800mah-6s-22-2v-50c-lipo-battery-with-ec3-connector.html</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/spektrum-1800mah-6s-22-2v-50c-smart-g2-lipo-battery-with-ic3-connector.html</t>
-  </si>
-  <si>
     <t>https://www.modelflight.com.au/dualsky-2200mah-6s-hed-lipo-battery-50c.html</t>
   </si>
   <si>
     <t>https://www.modelflight.com.au/dualsky-2700mah-6s-hed-lipo-battery-50c.html</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/dualsky-ultra-70-lipo-battery-2700mah-6s-70c.html</t>
-  </si>
-  <si>
     <t>Batteries w/o spec</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/dualsky-ultra-70-lipo-battery-2250mah-6s-70c.html</t>
-  </si>
-  <si>
-    <t>https://www.modelflight.com.au/spektrum-3200mah-6s-22-2v-100c-smart-g2-lipo-battery-with-ic5-connector.html</t>
-  </si>
-  <si>
-    <t>https://www.modelflight.com.au/spektrum-3200mah-6s-22-2v-smart-lipo-30c-ic5.html</t>
-  </si>
-  <si>
     <t>https://www.modelflight.com.au/dualsky-ultra-70-lipo-battery-3850mah-6s-70c.html</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/spektrum-3200mah-6s-22-2v-50c-smart-g2-lipo-battery-with-ic5-connector.html</t>
-  </si>
-  <si>
-    <t>https://www.modelflight.com.au/spektrum-3200mah-6s-22-2v-100c-smart-lipo-battery-ic3.html</t>
-  </si>
-  <si>
-    <t>https://www.modelflight.com.au/spektrum-3200mah-6s-22-2v-50c-smart-lipo-battery-ic3.html</t>
-  </si>
-  <si>
     <t>https://www.modelflight.com.au/dualsky-3700mah-6s-hed-lipo-battery-50c.html</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/spektrum-3200mah-6s-22-2v-30c-smart-g2-lipo-battery-with-ic5-connector.html</t>
-  </si>
-  <si>
     <t>https://www.modelflight.com.au/dualsky-3300mah-6s-hed-lipo-battery-50c.html</t>
   </si>
   <si>
@@ -137,9 +104,6 @@
     <t>https://www.modelflight.com.au/dualsky-4350mah-6s-hed-lipo-battery-50c.html</t>
   </si>
   <si>
-    <t>https://www.modelflight.com.au/dualsky-eco-s-lipo-battery-4000mah-6s-25c.html</t>
-  </si>
-  <si>
     <t>https://www.modelflight.com.au/dualsky-ultra-70-lipo-battery-4400mah-6s-70c.html</t>
   </si>
   <si>
@@ -147,9 +111,6 @@
   </si>
   <si>
     <t>https://www.modelflight.com.au/dualsky-eco-s-lipo-battery-5200mah-6s-25c.html</t>
-  </si>
-  <si>
-    <t>https://www.modelflight.com.au/prime-rc-5200mah-6s-22-2v-50c-lipo-battery-with-ec5-connector.html</t>
   </si>
   <si>
     <t>https://www.modelflight.com.au/dualsky-ultra-70-lipo-battery-5000mah-6s-70c.html</t>
@@ -570,20 +531,20 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.3984375" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -595,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -604,10 +565,10 @@
         <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1300</v>
       </c>
@@ -627,16 +588,16 @@
         <v>212</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="N2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1800</v>
       </c>
@@ -656,24 +617,24 @@
         <v>251</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1800</v>
+        <v>2200</v>
       </c>
       <c r="B4" s="1">
         <v>35</v>
       </c>
       <c r="C4" s="1">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1">
         <v>107</v>
@@ -682,160 +643,154 @@
         <v>6</v>
       </c>
       <c r="F4" s="1">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2700</v>
+      </c>
+      <c r="B5" s="1">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1">
+        <v>138</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1">
+        <v>392</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3200</v>
+      </c>
+      <c r="B6" s="1">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1">
+        <v>135</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>262</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>1800</v>
-      </c>
-      <c r="B5" s="1">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1">
-        <v>114</v>
-      </c>
-      <c r="E5" s="1">
-        <v>6</v>
-      </c>
-      <c r="F5" s="1">
-        <v>300</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>1800</v>
-      </c>
-      <c r="B6" s="1">
-        <v>35</v>
-      </c>
-      <c r="C6" s="1">
-        <v>42</v>
-      </c>
-      <c r="D6" s="1">
-        <v>108</v>
-      </c>
-      <c r="E6" s="1">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1">
-        <v>324</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N6" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3300</v>
+      </c>
+      <c r="B7" s="1">
+        <v>33</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1">
+        <v>140</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1">
+        <v>433</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>2200</v>
-      </c>
-      <c r="B7" s="1">
-        <v>35</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45</v>
-      </c>
-      <c r="D7" s="1">
-        <v>107</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1">
-        <v>325</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>2700</v>
+        <v>3700</v>
       </c>
       <c r="B8" s="1">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1">
         <v>44</v>
       </c>
       <c r="D8" s="1">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
       </c>
       <c r="F8" s="1">
-        <v>392</v>
+        <v>515</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>3200</v>
+        <v>3850</v>
       </c>
       <c r="B9" s="1">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E9" s="1">
         <v>6</v>
       </c>
       <c r="F9" s="1">
-        <v>262</v>
+        <v>594</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>3200</v>
+        <v>4000</v>
       </c>
       <c r="B10" s="1">
         <v>43</v>
       </c>
       <c r="C10" s="1">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1">
         <v>140</v>
@@ -844,252 +799,252 @@
         <v>6</v>
       </c>
       <c r="F10" s="1">
-        <v>430</v>
+        <v>580</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>3200</v>
+        <v>4200</v>
       </c>
       <c r="B11" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1">
+        <v>134</v>
+      </c>
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
+      <c r="F11" s="1">
+        <v>520</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4350</v>
+      </c>
+      <c r="B12" s="1">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1">
+        <v>47</v>
+      </c>
+      <c r="D12" s="1">
         <v>140</v>
       </c>
-      <c r="E11" s="1">
-        <v>6</v>
-      </c>
-      <c r="F11" s="1">
-        <v>460</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="E12" s="1">
+        <v>6</v>
+      </c>
+      <c r="F12" s="1">
+        <v>607</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4400</v>
+      </c>
+      <c r="B13" s="1">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1">
+        <v>160</v>
+      </c>
+      <c r="E13" s="1">
+        <v>6</v>
+      </c>
+      <c r="F13" s="1">
+        <v>698</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>3200</v>
-      </c>
-      <c r="B12" s="1">
-        <v>38</v>
-      </c>
-      <c r="C12" s="1">
-        <v>42</v>
-      </c>
-      <c r="D12" s="1">
-        <v>142</v>
-      </c>
-      <c r="E12" s="1">
-        <v>6</v>
-      </c>
-      <c r="F12" s="1">
-        <v>484</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>3200</v>
-      </c>
-      <c r="B13" s="1">
-        <v>42</v>
-      </c>
-      <c r="C13" s="1">
-        <v>38</v>
-      </c>
-      <c r="D13" s="1">
-        <v>141</v>
-      </c>
-      <c r="E13" s="1">
-        <v>6</v>
-      </c>
-      <c r="F13" s="1">
-        <v>490</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>3200</v>
+        <v>5000</v>
       </c>
       <c r="B14" s="1">
+        <v>46</v>
+      </c>
+      <c r="C14" s="1">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1">
+        <v>157</v>
+      </c>
+      <c r="E14" s="1">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1">
+        <v>791</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>5050</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44</v>
+      </c>
+      <c r="C15" s="1">
+        <v>54</v>
+      </c>
+      <c r="D15" s="1">
+        <v>140</v>
+      </c>
+      <c r="E15" s="1">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1">
+        <v>688</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>5200</v>
+      </c>
+      <c r="B16" s="1">
         <v>41</v>
       </c>
-      <c r="C14" s="1">
-        <v>43</v>
-      </c>
-      <c r="D14" s="1">
-        <v>142</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6</v>
-      </c>
-      <c r="F14" s="1">
-        <v>505</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
-        <v>3200</v>
-      </c>
-      <c r="B15" s="1">
-        <v>42</v>
-      </c>
-      <c r="C15" s="1">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1">
-        <v>142</v>
-      </c>
-      <c r="E15" s="1">
-        <v>6</v>
-      </c>
-      <c r="F15" s="1">
-        <v>515</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
-        <v>3300</v>
-      </c>
-      <c r="B16" s="1">
-        <v>33</v>
-      </c>
       <c r="C16" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="E16" s="1">
         <v>6</v>
       </c>
       <c r="F16" s="1">
-        <v>433</v>
+        <v>725</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>3700</v>
+        <v>5900</v>
       </c>
       <c r="B17" s="1">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="E17" s="1">
         <v>6</v>
       </c>
       <c r="F17" s="1">
-        <v>515</v>
+        <v>774</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>3850</v>
+        <v>6400</v>
       </c>
       <c r="B18" s="1">
         <v>45</v>
       </c>
       <c r="C18" s="1">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D18" s="1">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="E18" s="1">
         <v>6</v>
       </c>
       <c r="F18" s="1">
-        <v>594</v>
+        <v>805</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>4000</v>
+        <v>7200</v>
       </c>
       <c r="B19" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D19" s="1">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
       </c>
       <c r="F19" s="1">
-        <v>580</v>
+        <v>826</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>4000</v>
+        <v>8000</v>
       </c>
       <c r="B20" s="1">
         <v>42</v>
@@ -1098,514 +1053,322 @@
         <v>43</v>
       </c>
       <c r="D20" s="1">
-        <v>144</v>
+        <v>288</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
       </c>
       <c r="F20" s="1">
-        <v>580</v>
+        <v>1160</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>8400</v>
+      </c>
+      <c r="B21" s="1">
+        <v>86</v>
+      </c>
+      <c r="C21" s="1">
+        <v>88</v>
+      </c>
+      <c r="D21" s="1">
+        <v>268</v>
+      </c>
+      <c r="E21" s="1">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1040</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>8800</v>
+      </c>
+      <c r="B22" s="1">
+        <v>88</v>
+      </c>
+      <c r="C22" s="1">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1">
+        <v>320</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1396</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
-        <v>4000</v>
-      </c>
-      <c r="B21" s="1">
-        <v>37</v>
-      </c>
-      <c r="C21" s="1">
-        <v>44</v>
-      </c>
-      <c r="D21" s="1">
-        <v>135</v>
-      </c>
-      <c r="E21" s="1">
-        <v>6</v>
-      </c>
-      <c r="F21" s="1">
-        <v>582</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
-        <v>4200</v>
-      </c>
-      <c r="B22" s="1">
-        <v>43</v>
-      </c>
-      <c r="C22" s="1">
-        <v>44</v>
-      </c>
-      <c r="D22" s="1">
-        <v>134</v>
-      </c>
-      <c r="E22" s="1">
-        <v>6</v>
-      </c>
-      <c r="F22" s="1">
-        <v>520</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>4350</v>
+        <v>10000</v>
       </c>
       <c r="B23" s="1">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1">
-        <v>47</v>
+        <v>102</v>
       </c>
       <c r="D23" s="1">
-        <v>140</v>
+        <v>314</v>
       </c>
       <c r="E23" s="1">
         <v>6</v>
       </c>
       <c r="F23" s="1">
-        <v>607</v>
+        <v>1582</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>4400</v>
+        <v>10400</v>
       </c>
       <c r="B24" s="1">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C24" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="1">
-        <v>160</v>
+        <v>304</v>
       </c>
       <c r="E24" s="1">
         <v>6</v>
       </c>
       <c r="F24" s="1">
-        <v>698</v>
+        <v>1450</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>5000</v>
+        <v>11800</v>
       </c>
       <c r="B25" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1">
         <v>51</v>
       </c>
       <c r="D25" s="1">
-        <v>157</v>
+        <v>312</v>
       </c>
       <c r="E25" s="1">
         <v>6</v>
       </c>
       <c r="F25" s="1">
-        <v>791</v>
+        <v>1548</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>5050</v>
+        <v>12800</v>
       </c>
       <c r="B26" s="1">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D26" s="1">
-        <v>140</v>
+        <v>312</v>
       </c>
       <c r="E26" s="1">
         <v>6</v>
       </c>
       <c r="F26" s="1">
-        <v>688</v>
+        <v>1610</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>5200</v>
+        <v>14400</v>
       </c>
       <c r="B27" s="1">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="D27" s="1">
-        <v>152</v>
+        <v>306</v>
       </c>
       <c r="E27" s="1">
         <v>6</v>
       </c>
       <c r="F27" s="1">
-        <v>725</v>
+        <v>826</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
-        <v>5200</v>
-      </c>
-      <c r="B28" s="1">
-        <v>44</v>
-      </c>
-      <c r="C28" s="1">
-        <v>50</v>
-      </c>
-      <c r="D28" s="1">
-        <v>153</v>
-      </c>
-      <c r="E28" s="1">
-        <v>6</v>
-      </c>
-      <c r="F28" s="1">
-        <v>765</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="1">
-        <v>5900</v>
-      </c>
-      <c r="B29" s="1">
-        <v>45</v>
-      </c>
-      <c r="C29" s="1">
-        <v>51</v>
-      </c>
-      <c r="D29" s="1">
-        <v>156</v>
-      </c>
-      <c r="E29" s="1">
-        <v>6</v>
-      </c>
-      <c r="F29" s="1">
-        <v>774</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
-        <v>6400</v>
-      </c>
-      <c r="B30" s="1">
-        <v>45</v>
-      </c>
-      <c r="C30" s="1">
-        <v>52</v>
-      </c>
-      <c r="D30" s="1">
-        <v>156</v>
-      </c>
-      <c r="E30" s="1">
-        <v>6</v>
-      </c>
-      <c r="F30" s="1">
-        <v>805</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" s="1">
-        <v>7200</v>
-      </c>
-      <c r="B31" s="1">
-        <v>45</v>
-      </c>
-      <c r="C31" s="1">
-        <v>53</v>
-      </c>
-      <c r="D31" s="1">
-        <v>153</v>
-      </c>
-      <c r="E31" s="1">
-        <v>6</v>
-      </c>
-      <c r="F31" s="1">
-        <v>826</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
-        <v>8000</v>
-      </c>
-      <c r="B32" s="1">
-        <v>42</v>
-      </c>
-      <c r="C32" s="1">
-        <v>43</v>
-      </c>
-      <c r="D32" s="1">
-        <v>288</v>
-      </c>
-      <c r="E32" s="1">
-        <v>6</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1160</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
-        <v>8400</v>
-      </c>
-      <c r="B33" s="1">
-        <v>86</v>
-      </c>
-      <c r="C33" s="1">
-        <v>88</v>
-      </c>
-      <c r="D33" s="1">
-        <v>268</v>
-      </c>
-      <c r="E33" s="1">
-        <v>6</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1040</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
-        <v>8800</v>
-      </c>
-      <c r="B34" s="1">
-        <v>88</v>
-      </c>
-      <c r="C34" s="1">
-        <v>46</v>
-      </c>
-      <c r="D34" s="1">
-        <v>320</v>
-      </c>
-      <c r="E34" s="1">
-        <v>6</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1396</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
-        <v>10000</v>
-      </c>
-      <c r="B35" s="1">
-        <v>46</v>
-      </c>
-      <c r="C35" s="1">
-        <v>102</v>
-      </c>
-      <c r="D35" s="1">
-        <v>314</v>
-      </c>
-      <c r="E35" s="1">
-        <v>6</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1582</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
-        <v>10400</v>
-      </c>
-      <c r="B36" s="1">
-        <v>82</v>
-      </c>
-      <c r="C36" s="1">
-        <v>45</v>
-      </c>
-      <c r="D36" s="1">
-        <v>304</v>
-      </c>
-      <c r="E36" s="1">
-        <v>6</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1450</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A37" s="1">
-        <v>11800</v>
-      </c>
-      <c r="B37" s="1">
-        <v>45</v>
-      </c>
-      <c r="C37" s="1">
-        <v>51</v>
-      </c>
-      <c r="D37" s="1">
-        <v>312</v>
-      </c>
-      <c r="E37" s="1">
-        <v>6</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1548</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="1">
-        <v>12800</v>
-      </c>
-      <c r="B38" s="1">
-        <v>45</v>
-      </c>
-      <c r="C38" s="1">
-        <v>52</v>
-      </c>
-      <c r="D38" s="1">
-        <v>312</v>
-      </c>
-      <c r="E38" s="1">
-        <v>6</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1610</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="1">
-        <v>14400</v>
-      </c>
-      <c r="B39" s="1">
-        <v>45</v>
-      </c>
-      <c r="C39" s="1">
-        <v>53</v>
-      </c>
-      <c r="D39" s="1">
-        <v>306</v>
-      </c>
-      <c r="E39" s="1">
-        <v>6</v>
-      </c>
-      <c r="F39" s="1">
-        <v>826</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1613,6 +1376,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7B4AA51A86DF64F8EEA3B7ACC01600E" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="37503d37778738f9b8e5b50734e360b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5f869584-441e-42c5-8d1e-76b11125194b" xmlns:ns3="9df0515c-157b-471a-a0ef-89af1efb2dd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7f630545ba42abbb2436d67874f362a0" ns2:_="" ns3:_="">
     <xsd:import namespace="5f869584-441e-42c5-8d1e-76b11125194b"/>
@@ -1835,15 +1607,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1856,6 +1619,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A79501D-A641-46E9-8090-FFC728BDED2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB9A91A5-3E46-403A-B8FE-FB78FF3ACF94}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1874,14 +1645,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A79501D-A641-46E9-8090-FFC728BDED2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E24B1721-9C5D-41CC-823C-A30077D27BE1}">
   <ds:schemaRefs>

</xml_diff>